<commit_message>
Edited nmt stats file
</commit_message>
<xml_diff>
--- a/nmt/астатистика/nmt.0.saria.xlsx
+++ b/nmt/астатистика/nmt.0.saria.xlsx
@@ -42,8 +42,9 @@
 Спасибо за помощь!</t>
   </si>
   <si>
-    <t xml:space="preserve">A: агхақәа маҷуп, аҵакы еилкаауп.
-B: агхақәа рацәоуп, аҵакы хәҭак иҟоуп.
+    <t xml:space="preserve">A: гхак ыҟоуп.
+B: агхақәа рацәоуп, аха 
+аҵакы еилкаауп.
 C: иашаӡам акагьы.</t>
   </si>
   <si>
@@ -1450,7 +1451,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1501,6 +1502,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1645,10 +1650,10 @@
   <dimension ref="A1:F1008"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="118" zoomScaleNormal="118" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.89"/>
@@ -4152,2404 +4157,2404 @@
       </c>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C209" s="13"/>
+      <c r="C209" s="14"/>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C210" s="13"/>
+      <c r="C210" s="14"/>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C211" s="13"/>
+      <c r="C211" s="14"/>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C212" s="13"/>
+      <c r="C212" s="14"/>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C213" s="13"/>
+      <c r="C213" s="14"/>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C214" s="13"/>
+      <c r="C214" s="14"/>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C215" s="13"/>
+      <c r="C215" s="14"/>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C216" s="13"/>
+      <c r="C216" s="14"/>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C217" s="13"/>
+      <c r="C217" s="14"/>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C218" s="13"/>
+      <c r="C218" s="14"/>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C219" s="13"/>
+      <c r="C219" s="14"/>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C220" s="13"/>
+      <c r="C220" s="14"/>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C221" s="13"/>
+      <c r="C221" s="14"/>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C222" s="13"/>
+      <c r="C222" s="14"/>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C223" s="13"/>
+      <c r="C223" s="14"/>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C224" s="13"/>
+      <c r="C224" s="14"/>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C225" s="13"/>
+      <c r="C225" s="14"/>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C226" s="13"/>
+      <c r="C226" s="14"/>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C227" s="13"/>
+      <c r="C227" s="14"/>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C228" s="13"/>
+      <c r="C228" s="14"/>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C229" s="13"/>
+      <c r="C229" s="14"/>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C230" s="13"/>
+      <c r="C230" s="14"/>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C231" s="13"/>
+      <c r="C231" s="14"/>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C232" s="13"/>
+      <c r="C232" s="14"/>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C233" s="13"/>
+      <c r="C233" s="14"/>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C234" s="13"/>
+      <c r="C234" s="14"/>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C235" s="13"/>
+      <c r="C235" s="14"/>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C236" s="13"/>
+      <c r="C236" s="14"/>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C237" s="13"/>
+      <c r="C237" s="14"/>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C238" s="13"/>
+      <c r="C238" s="14"/>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C239" s="13"/>
+      <c r="C239" s="14"/>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C240" s="13"/>
+      <c r="C240" s="14"/>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C241" s="13"/>
+      <c r="C241" s="14"/>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C242" s="13"/>
+      <c r="C242" s="14"/>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C243" s="13"/>
+      <c r="C243" s="14"/>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C244" s="13"/>
+      <c r="C244" s="14"/>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C245" s="13"/>
+      <c r="C245" s="14"/>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C246" s="13"/>
+      <c r="C246" s="14"/>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C247" s="13"/>
+      <c r="C247" s="14"/>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C248" s="13"/>
+      <c r="C248" s="14"/>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C249" s="13"/>
+      <c r="C249" s="14"/>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C250" s="13"/>
+      <c r="C250" s="14"/>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C251" s="13"/>
+      <c r="C251" s="14"/>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C252" s="13"/>
+      <c r="C252" s="14"/>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C253" s="13"/>
+      <c r="C253" s="14"/>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C254" s="13"/>
+      <c r="C254" s="14"/>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C255" s="13"/>
+      <c r="C255" s="14"/>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C256" s="13"/>
+      <c r="C256" s="14"/>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C257" s="13"/>
+      <c r="C257" s="14"/>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C258" s="13"/>
+      <c r="C258" s="14"/>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C259" s="13"/>
+      <c r="C259" s="14"/>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C260" s="13"/>
+      <c r="C260" s="14"/>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C261" s="13"/>
+      <c r="C261" s="14"/>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C262" s="13"/>
+      <c r="C262" s="14"/>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C263" s="13"/>
+      <c r="C263" s="14"/>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C264" s="13"/>
+      <c r="C264" s="14"/>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C265" s="13"/>
+      <c r="C265" s="14"/>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C266" s="13"/>
+      <c r="C266" s="14"/>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C267" s="13"/>
+      <c r="C267" s="14"/>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C268" s="13"/>
+      <c r="C268" s="14"/>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C269" s="13"/>
+      <c r="C269" s="14"/>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C270" s="13"/>
+      <c r="C270" s="14"/>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C271" s="13"/>
+      <c r="C271" s="14"/>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C272" s="13"/>
+      <c r="C272" s="14"/>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C273" s="13"/>
+      <c r="C273" s="14"/>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C274" s="13"/>
+      <c r="C274" s="14"/>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C275" s="13"/>
+      <c r="C275" s="14"/>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C276" s="13"/>
+      <c r="C276" s="14"/>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C277" s="13"/>
+      <c r="C277" s="14"/>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C278" s="13"/>
+      <c r="C278" s="14"/>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C279" s="13"/>
+      <c r="C279" s="14"/>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C280" s="13"/>
+      <c r="C280" s="14"/>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C281" s="13"/>
+      <c r="C281" s="14"/>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C282" s="13"/>
+      <c r="C282" s="14"/>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C283" s="13"/>
+      <c r="C283" s="14"/>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C284" s="13"/>
+      <c r="C284" s="14"/>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C285" s="13"/>
+      <c r="C285" s="14"/>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C286" s="13"/>
+      <c r="C286" s="14"/>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C287" s="13"/>
+      <c r="C287" s="14"/>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C288" s="13"/>
+      <c r="C288" s="14"/>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C289" s="13"/>
+      <c r="C289" s="14"/>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C290" s="13"/>
+      <c r="C290" s="14"/>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C291" s="13"/>
+      <c r="C291" s="14"/>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C292" s="13"/>
+      <c r="C292" s="14"/>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C293" s="13"/>
+      <c r="C293" s="14"/>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C294" s="13"/>
+      <c r="C294" s="14"/>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C295" s="13"/>
+      <c r="C295" s="14"/>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C296" s="13"/>
+      <c r="C296" s="14"/>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C297" s="13"/>
+      <c r="C297" s="14"/>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C298" s="13"/>
+      <c r="C298" s="14"/>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C299" s="13"/>
+      <c r="C299" s="14"/>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C300" s="13"/>
+      <c r="C300" s="14"/>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C301" s="13"/>
+      <c r="C301" s="14"/>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C302" s="13"/>
+      <c r="C302" s="14"/>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C303" s="13"/>
+      <c r="C303" s="14"/>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C304" s="13"/>
+      <c r="C304" s="14"/>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C305" s="13"/>
+      <c r="C305" s="14"/>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C306" s="13"/>
+      <c r="C306" s="14"/>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C307" s="13"/>
+      <c r="C307" s="14"/>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C308" s="13"/>
+      <c r="C308" s="14"/>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C309" s="13"/>
+      <c r="C309" s="14"/>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C310" s="13"/>
+      <c r="C310" s="14"/>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C311" s="13"/>
+      <c r="C311" s="14"/>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C312" s="13"/>
+      <c r="C312" s="14"/>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C313" s="13"/>
+      <c r="C313" s="14"/>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C314" s="13"/>
+      <c r="C314" s="14"/>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C315" s="13"/>
+      <c r="C315" s="14"/>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C316" s="13"/>
+      <c r="C316" s="14"/>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C317" s="13"/>
+      <c r="C317" s="14"/>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C318" s="13"/>
+      <c r="C318" s="14"/>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C319" s="13"/>
+      <c r="C319" s="14"/>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C320" s="13"/>
+      <c r="C320" s="14"/>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C321" s="13"/>
+      <c r="C321" s="14"/>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C322" s="13"/>
+      <c r="C322" s="14"/>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C323" s="13"/>
+      <c r="C323" s="14"/>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C324" s="13"/>
+      <c r="C324" s="14"/>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C325" s="13"/>
+      <c r="C325" s="14"/>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C326" s="13"/>
+      <c r="C326" s="14"/>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C327" s="13"/>
+      <c r="C327" s="14"/>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C328" s="13"/>
+      <c r="C328" s="14"/>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C329" s="13"/>
+      <c r="C329" s="14"/>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C330" s="13"/>
+      <c r="C330" s="14"/>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C331" s="13"/>
+      <c r="C331" s="14"/>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C332" s="13"/>
+      <c r="C332" s="14"/>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C333" s="13"/>
+      <c r="C333" s="14"/>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C334" s="13"/>
+      <c r="C334" s="14"/>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C335" s="13"/>
+      <c r="C335" s="14"/>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C336" s="13"/>
+      <c r="C336" s="14"/>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C337" s="13"/>
+      <c r="C337" s="14"/>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C338" s="13"/>
+      <c r="C338" s="14"/>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C339" s="13"/>
+      <c r="C339" s="14"/>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C340" s="13"/>
+      <c r="C340" s="14"/>
     </row>
     <row r="341" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C341" s="13"/>
+      <c r="C341" s="14"/>
     </row>
     <row r="342" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C342" s="13"/>
+      <c r="C342" s="14"/>
     </row>
     <row r="343" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C343" s="13"/>
+      <c r="C343" s="14"/>
     </row>
     <row r="344" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C344" s="13"/>
+      <c r="C344" s="14"/>
     </row>
     <row r="345" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C345" s="13"/>
+      <c r="C345" s="14"/>
     </row>
     <row r="346" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C346" s="13"/>
+      <c r="C346" s="14"/>
     </row>
     <row r="347" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C347" s="13"/>
+      <c r="C347" s="14"/>
     </row>
     <row r="348" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C348" s="13"/>
+      <c r="C348" s="14"/>
     </row>
     <row r="349" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C349" s="13"/>
+      <c r="C349" s="14"/>
     </row>
     <row r="350" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C350" s="13"/>
+      <c r="C350" s="14"/>
     </row>
     <row r="351" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C351" s="13"/>
+      <c r="C351" s="14"/>
     </row>
     <row r="352" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C352" s="13"/>
+      <c r="C352" s="14"/>
     </row>
     <row r="353" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C353" s="13"/>
+      <c r="C353" s="14"/>
     </row>
     <row r="354" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C354" s="13"/>
+      <c r="C354" s="14"/>
     </row>
     <row r="355" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C355" s="13"/>
+      <c r="C355" s="14"/>
     </row>
     <row r="356" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C356" s="13"/>
+      <c r="C356" s="14"/>
     </row>
     <row r="357" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C357" s="13"/>
+      <c r="C357" s="14"/>
     </row>
     <row r="358" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C358" s="13"/>
+      <c r="C358" s="14"/>
     </row>
     <row r="359" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C359" s="13"/>
+      <c r="C359" s="14"/>
     </row>
     <row r="360" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C360" s="13"/>
+      <c r="C360" s="14"/>
     </row>
     <row r="361" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C361" s="13"/>
+      <c r="C361" s="14"/>
     </row>
     <row r="362" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C362" s="13"/>
+      <c r="C362" s="14"/>
     </row>
     <row r="363" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C363" s="13"/>
+      <c r="C363" s="14"/>
     </row>
     <row r="364" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C364" s="13"/>
+      <c r="C364" s="14"/>
     </row>
     <row r="365" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C365" s="13"/>
+      <c r="C365" s="14"/>
     </row>
     <row r="366" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C366" s="13"/>
+      <c r="C366" s="14"/>
     </row>
     <row r="367" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C367" s="13"/>
+      <c r="C367" s="14"/>
     </row>
     <row r="368" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C368" s="13"/>
+      <c r="C368" s="14"/>
     </row>
     <row r="369" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C369" s="13"/>
+      <c r="C369" s="14"/>
     </row>
     <row r="370" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C370" s="13"/>
+      <c r="C370" s="14"/>
     </row>
     <row r="371" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C371" s="13"/>
+      <c r="C371" s="14"/>
     </row>
     <row r="372" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C372" s="13"/>
+      <c r="C372" s="14"/>
     </row>
     <row r="373" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C373" s="13"/>
+      <c r="C373" s="14"/>
     </row>
     <row r="374" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C374" s="13"/>
+      <c r="C374" s="14"/>
     </row>
     <row r="375" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C375" s="13"/>
+      <c r="C375" s="14"/>
     </row>
     <row r="376" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C376" s="13"/>
+      <c r="C376" s="14"/>
     </row>
     <row r="377" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C377" s="13"/>
+      <c r="C377" s="14"/>
     </row>
     <row r="378" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C378" s="13"/>
+      <c r="C378" s="14"/>
     </row>
     <row r="379" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C379" s="13"/>
+      <c r="C379" s="14"/>
     </row>
     <row r="380" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C380" s="13"/>
+      <c r="C380" s="14"/>
     </row>
     <row r="381" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C381" s="13"/>
+      <c r="C381" s="14"/>
     </row>
     <row r="382" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C382" s="13"/>
+      <c r="C382" s="14"/>
     </row>
     <row r="383" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C383" s="13"/>
+      <c r="C383" s="14"/>
     </row>
     <row r="384" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C384" s="13"/>
+      <c r="C384" s="14"/>
     </row>
     <row r="385" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C385" s="13"/>
+      <c r="C385" s="14"/>
     </row>
     <row r="386" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C386" s="13"/>
+      <c r="C386" s="14"/>
     </row>
     <row r="387" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C387" s="13"/>
+      <c r="C387" s="14"/>
     </row>
     <row r="388" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C388" s="13"/>
+      <c r="C388" s="14"/>
     </row>
     <row r="389" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C389" s="13"/>
+      <c r="C389" s="14"/>
     </row>
     <row r="390" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C390" s="13"/>
+      <c r="C390" s="14"/>
     </row>
     <row r="391" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C391" s="13"/>
+      <c r="C391" s="14"/>
     </row>
     <row r="392" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C392" s="13"/>
+      <c r="C392" s="14"/>
     </row>
     <row r="393" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C393" s="13"/>
+      <c r="C393" s="14"/>
     </row>
     <row r="394" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C394" s="13"/>
+      <c r="C394" s="14"/>
     </row>
     <row r="395" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C395" s="13"/>
+      <c r="C395" s="14"/>
     </row>
     <row r="396" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C396" s="13"/>
+      <c r="C396" s="14"/>
     </row>
     <row r="397" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C397" s="13"/>
+      <c r="C397" s="14"/>
     </row>
     <row r="398" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C398" s="13"/>
+      <c r="C398" s="14"/>
     </row>
     <row r="399" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C399" s="13"/>
+      <c r="C399" s="14"/>
     </row>
     <row r="400" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C400" s="13"/>
+      <c r="C400" s="14"/>
     </row>
     <row r="401" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C401" s="13"/>
+      <c r="C401" s="14"/>
     </row>
     <row r="402" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C402" s="13"/>
+      <c r="C402" s="14"/>
     </row>
     <row r="403" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C403" s="13"/>
+      <c r="C403" s="14"/>
     </row>
     <row r="404" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C404" s="13"/>
+      <c r="C404" s="14"/>
     </row>
     <row r="405" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C405" s="13"/>
+      <c r="C405" s="14"/>
     </row>
     <row r="406" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C406" s="13"/>
+      <c r="C406" s="14"/>
     </row>
     <row r="407" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C407" s="13"/>
+      <c r="C407" s="14"/>
     </row>
     <row r="408" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C408" s="13"/>
+      <c r="C408" s="14"/>
     </row>
     <row r="409" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C409" s="13"/>
+      <c r="C409" s="14"/>
     </row>
     <row r="410" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C410" s="13"/>
+      <c r="C410" s="14"/>
     </row>
     <row r="411" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C411" s="13"/>
+      <c r="C411" s="14"/>
     </row>
     <row r="412" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C412" s="13"/>
+      <c r="C412" s="14"/>
     </row>
     <row r="413" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C413" s="13"/>
+      <c r="C413" s="14"/>
     </row>
     <row r="414" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C414" s="13"/>
+      <c r="C414" s="14"/>
     </row>
     <row r="415" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C415" s="13"/>
+      <c r="C415" s="14"/>
     </row>
     <row r="416" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C416" s="13"/>
+      <c r="C416" s="14"/>
     </row>
     <row r="417" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C417" s="13"/>
+      <c r="C417" s="14"/>
     </row>
     <row r="418" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C418" s="13"/>
+      <c r="C418" s="14"/>
     </row>
     <row r="419" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C419" s="13"/>
+      <c r="C419" s="14"/>
     </row>
     <row r="420" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C420" s="13"/>
+      <c r="C420" s="14"/>
     </row>
     <row r="421" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C421" s="13"/>
+      <c r="C421" s="14"/>
     </row>
     <row r="422" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C422" s="13"/>
+      <c r="C422" s="14"/>
     </row>
     <row r="423" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C423" s="13"/>
+      <c r="C423" s="14"/>
     </row>
     <row r="424" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C424" s="13"/>
+      <c r="C424" s="14"/>
     </row>
     <row r="425" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C425" s="13"/>
+      <c r="C425" s="14"/>
     </row>
     <row r="426" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C426" s="13"/>
+      <c r="C426" s="14"/>
     </row>
     <row r="427" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C427" s="13"/>
+      <c r="C427" s="14"/>
     </row>
     <row r="428" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="13"/>
+      <c r="C428" s="14"/>
     </row>
     <row r="429" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C429" s="13"/>
+      <c r="C429" s="14"/>
     </row>
     <row r="430" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C430" s="13"/>
+      <c r="C430" s="14"/>
     </row>
     <row r="431" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C431" s="13"/>
+      <c r="C431" s="14"/>
     </row>
     <row r="432" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C432" s="13"/>
+      <c r="C432" s="14"/>
     </row>
     <row r="433" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C433" s="13"/>
+      <c r="C433" s="14"/>
     </row>
     <row r="434" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C434" s="13"/>
+      <c r="C434" s="14"/>
     </row>
     <row r="435" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C435" s="13"/>
+      <c r="C435" s="14"/>
     </row>
     <row r="436" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C436" s="13"/>
+      <c r="C436" s="14"/>
     </row>
     <row r="437" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C437" s="13"/>
+      <c r="C437" s="14"/>
     </row>
     <row r="438" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C438" s="13"/>
+      <c r="C438" s="14"/>
     </row>
     <row r="439" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C439" s="13"/>
+      <c r="C439" s="14"/>
     </row>
     <row r="440" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C440" s="13"/>
+      <c r="C440" s="14"/>
     </row>
     <row r="441" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C441" s="13"/>
+      <c r="C441" s="14"/>
     </row>
     <row r="442" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C442" s="13"/>
+      <c r="C442" s="14"/>
     </row>
     <row r="443" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C443" s="13"/>
+      <c r="C443" s="14"/>
     </row>
     <row r="444" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C444" s="13"/>
+      <c r="C444" s="14"/>
     </row>
     <row r="445" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C445" s="13"/>
+      <c r="C445" s="14"/>
     </row>
     <row r="446" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C446" s="13"/>
+      <c r="C446" s="14"/>
     </row>
     <row r="447" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C447" s="13"/>
+      <c r="C447" s="14"/>
     </row>
     <row r="448" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C448" s="13"/>
+      <c r="C448" s="14"/>
     </row>
     <row r="449" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C449" s="13"/>
+      <c r="C449" s="14"/>
     </row>
     <row r="450" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C450" s="13"/>
+      <c r="C450" s="14"/>
     </row>
     <row r="451" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C451" s="13"/>
+      <c r="C451" s="14"/>
     </row>
     <row r="452" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C452" s="13"/>
+      <c r="C452" s="14"/>
     </row>
     <row r="453" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C453" s="13"/>
+      <c r="C453" s="14"/>
     </row>
     <row r="454" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C454" s="13"/>
+      <c r="C454" s="14"/>
     </row>
     <row r="455" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C455" s="13"/>
+      <c r="C455" s="14"/>
     </row>
     <row r="456" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C456" s="13"/>
+      <c r="C456" s="14"/>
     </row>
     <row r="457" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C457" s="13"/>
+      <c r="C457" s="14"/>
     </row>
     <row r="458" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C458" s="13"/>
+      <c r="C458" s="14"/>
     </row>
     <row r="459" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C459" s="13"/>
+      <c r="C459" s="14"/>
     </row>
     <row r="460" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C460" s="13"/>
+      <c r="C460" s="14"/>
     </row>
     <row r="461" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C461" s="13"/>
+      <c r="C461" s="14"/>
     </row>
     <row r="462" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C462" s="13"/>
+      <c r="C462" s="14"/>
     </row>
     <row r="463" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C463" s="13"/>
+      <c r="C463" s="14"/>
     </row>
     <row r="464" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C464" s="13"/>
+      <c r="C464" s="14"/>
     </row>
     <row r="465" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C465" s="13"/>
+      <c r="C465" s="14"/>
     </row>
     <row r="466" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C466" s="13"/>
+      <c r="C466" s="14"/>
     </row>
     <row r="467" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C467" s="13"/>
+      <c r="C467" s="14"/>
     </row>
     <row r="468" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C468" s="13"/>
+      <c r="C468" s="14"/>
     </row>
     <row r="469" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C469" s="13"/>
+      <c r="C469" s="14"/>
     </row>
     <row r="470" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C470" s="13"/>
+      <c r="C470" s="14"/>
     </row>
     <row r="471" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C471" s="13"/>
+      <c r="C471" s="14"/>
     </row>
     <row r="472" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C472" s="13"/>
+      <c r="C472" s="14"/>
     </row>
     <row r="473" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C473" s="13"/>
+      <c r="C473" s="14"/>
     </row>
     <row r="474" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C474" s="13"/>
+      <c r="C474" s="14"/>
     </row>
     <row r="475" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C475" s="13"/>
+      <c r="C475" s="14"/>
     </row>
     <row r="476" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C476" s="13"/>
+      <c r="C476" s="14"/>
     </row>
     <row r="477" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C477" s="13"/>
+      <c r="C477" s="14"/>
     </row>
     <row r="478" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C478" s="13"/>
+      <c r="C478" s="14"/>
     </row>
     <row r="479" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C479" s="13"/>
+      <c r="C479" s="14"/>
     </row>
     <row r="480" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C480" s="13"/>
+      <c r="C480" s="14"/>
     </row>
     <row r="481" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C481" s="13"/>
+      <c r="C481" s="14"/>
     </row>
     <row r="482" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C482" s="13"/>
+      <c r="C482" s="14"/>
     </row>
     <row r="483" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C483" s="13"/>
+      <c r="C483" s="14"/>
     </row>
     <row r="484" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C484" s="13"/>
+      <c r="C484" s="14"/>
     </row>
     <row r="485" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C485" s="13"/>
+      <c r="C485" s="14"/>
     </row>
     <row r="486" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C486" s="13"/>
+      <c r="C486" s="14"/>
     </row>
     <row r="487" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C487" s="13"/>
+      <c r="C487" s="14"/>
     </row>
     <row r="488" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C488" s="13"/>
+      <c r="C488" s="14"/>
     </row>
     <row r="489" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C489" s="13"/>
+      <c r="C489" s="14"/>
     </row>
     <row r="490" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C490" s="13"/>
+      <c r="C490" s="14"/>
     </row>
     <row r="491" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C491" s="13"/>
+      <c r="C491" s="14"/>
     </row>
     <row r="492" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C492" s="13"/>
+      <c r="C492" s="14"/>
     </row>
     <row r="493" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C493" s="13"/>
+      <c r="C493" s="14"/>
     </row>
     <row r="494" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C494" s="13"/>
+      <c r="C494" s="14"/>
     </row>
     <row r="495" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C495" s="13"/>
+      <c r="C495" s="14"/>
     </row>
     <row r="496" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C496" s="13"/>
+      <c r="C496" s="14"/>
     </row>
     <row r="497" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C497" s="13"/>
+      <c r="C497" s="14"/>
     </row>
     <row r="498" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C498" s="13"/>
+      <c r="C498" s="14"/>
     </row>
     <row r="499" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C499" s="13"/>
+      <c r="C499" s="14"/>
     </row>
     <row r="500" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C500" s="13"/>
+      <c r="C500" s="14"/>
     </row>
     <row r="501" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C501" s="13"/>
+      <c r="C501" s="14"/>
     </row>
     <row r="502" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C502" s="13"/>
+      <c r="C502" s="14"/>
     </row>
     <row r="503" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C503" s="13"/>
+      <c r="C503" s="14"/>
     </row>
     <row r="504" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C504" s="13"/>
+      <c r="C504" s="14"/>
     </row>
     <row r="505" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C505" s="13"/>
+      <c r="C505" s="14"/>
     </row>
     <row r="506" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C506" s="13"/>
+      <c r="C506" s="14"/>
     </row>
     <row r="507" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C507" s="13"/>
+      <c r="C507" s="14"/>
     </row>
     <row r="508" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C508" s="13"/>
+      <c r="C508" s="14"/>
     </row>
     <row r="509" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C509" s="13"/>
+      <c r="C509" s="14"/>
     </row>
     <row r="510" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C510" s="13"/>
+      <c r="C510" s="14"/>
     </row>
     <row r="511" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C511" s="13"/>
+      <c r="C511" s="14"/>
     </row>
     <row r="512" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C512" s="13"/>
+      <c r="C512" s="14"/>
     </row>
     <row r="513" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C513" s="13"/>
+      <c r="C513" s="14"/>
     </row>
     <row r="514" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C514" s="13"/>
+      <c r="C514" s="14"/>
     </row>
     <row r="515" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C515" s="13"/>
+      <c r="C515" s="14"/>
     </row>
     <row r="516" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C516" s="13"/>
+      <c r="C516" s="14"/>
     </row>
     <row r="517" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C517" s="13"/>
+      <c r="C517" s="14"/>
     </row>
     <row r="518" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C518" s="13"/>
+      <c r="C518" s="14"/>
     </row>
     <row r="519" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C519" s="13"/>
+      <c r="C519" s="14"/>
     </row>
     <row r="520" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C520" s="13"/>
+      <c r="C520" s="14"/>
     </row>
     <row r="521" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C521" s="13"/>
+      <c r="C521" s="14"/>
     </row>
     <row r="522" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C522" s="13"/>
+      <c r="C522" s="14"/>
     </row>
     <row r="523" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C523" s="13"/>
+      <c r="C523" s="14"/>
     </row>
     <row r="524" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C524" s="13"/>
+      <c r="C524" s="14"/>
     </row>
     <row r="525" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C525" s="13"/>
+      <c r="C525" s="14"/>
     </row>
     <row r="526" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C526" s="13"/>
+      <c r="C526" s="14"/>
     </row>
     <row r="527" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C527" s="13"/>
+      <c r="C527" s="14"/>
     </row>
     <row r="528" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C528" s="13"/>
+      <c r="C528" s="14"/>
     </row>
     <row r="529" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C529" s="13"/>
+      <c r="C529" s="14"/>
     </row>
     <row r="530" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C530" s="13"/>
+      <c r="C530" s="14"/>
     </row>
     <row r="531" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C531" s="13"/>
+      <c r="C531" s="14"/>
     </row>
     <row r="532" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C532" s="13"/>
+      <c r="C532" s="14"/>
     </row>
     <row r="533" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C533" s="13"/>
+      <c r="C533" s="14"/>
     </row>
     <row r="534" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C534" s="13"/>
+      <c r="C534" s="14"/>
     </row>
     <row r="535" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C535" s="13"/>
+      <c r="C535" s="14"/>
     </row>
     <row r="536" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C536" s="13"/>
+      <c r="C536" s="14"/>
     </row>
     <row r="537" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C537" s="13"/>
+      <c r="C537" s="14"/>
     </row>
     <row r="538" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C538" s="13"/>
+      <c r="C538" s="14"/>
     </row>
     <row r="539" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C539" s="13"/>
+      <c r="C539" s="14"/>
     </row>
     <row r="540" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C540" s="13"/>
+      <c r="C540" s="14"/>
     </row>
     <row r="541" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C541" s="13"/>
+      <c r="C541" s="14"/>
     </row>
     <row r="542" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C542" s="13"/>
+      <c r="C542" s="14"/>
     </row>
     <row r="543" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C543" s="13"/>
+      <c r="C543" s="14"/>
     </row>
     <row r="544" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C544" s="13"/>
+      <c r="C544" s="14"/>
     </row>
     <row r="545" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C545" s="13"/>
+      <c r="C545" s="14"/>
     </row>
     <row r="546" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C546" s="13"/>
+      <c r="C546" s="14"/>
     </row>
     <row r="547" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C547" s="13"/>
+      <c r="C547" s="14"/>
     </row>
     <row r="548" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C548" s="13"/>
+      <c r="C548" s="14"/>
     </row>
     <row r="549" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C549" s="13"/>
+      <c r="C549" s="14"/>
     </row>
     <row r="550" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C550" s="13"/>
+      <c r="C550" s="14"/>
     </row>
     <row r="551" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C551" s="13"/>
+      <c r="C551" s="14"/>
     </row>
     <row r="552" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C552" s="13"/>
+      <c r="C552" s="14"/>
     </row>
     <row r="553" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C553" s="13"/>
+      <c r="C553" s="14"/>
     </row>
     <row r="554" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C554" s="13"/>
+      <c r="C554" s="14"/>
     </row>
     <row r="555" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C555" s="13"/>
+      <c r="C555" s="14"/>
     </row>
     <row r="556" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C556" s="13"/>
+      <c r="C556" s="14"/>
     </row>
     <row r="557" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C557" s="13"/>
+      <c r="C557" s="14"/>
     </row>
     <row r="558" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C558" s="13"/>
+      <c r="C558" s="14"/>
     </row>
     <row r="559" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C559" s="13"/>
+      <c r="C559" s="14"/>
     </row>
     <row r="560" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C560" s="13"/>
+      <c r="C560" s="14"/>
     </row>
     <row r="561" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C561" s="13"/>
+      <c r="C561" s="14"/>
     </row>
     <row r="562" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C562" s="13"/>
+      <c r="C562" s="14"/>
     </row>
     <row r="563" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C563" s="13"/>
+      <c r="C563" s="14"/>
     </row>
     <row r="564" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C564" s="13"/>
+      <c r="C564" s="14"/>
     </row>
     <row r="565" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C565" s="13"/>
+      <c r="C565" s="14"/>
     </row>
     <row r="566" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C566" s="13"/>
+      <c r="C566" s="14"/>
     </row>
     <row r="567" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C567" s="13"/>
+      <c r="C567" s="14"/>
     </row>
     <row r="568" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C568" s="13"/>
+      <c r="C568" s="14"/>
     </row>
     <row r="569" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C569" s="13"/>
+      <c r="C569" s="14"/>
     </row>
     <row r="570" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C570" s="13"/>
+      <c r="C570" s="14"/>
     </row>
     <row r="571" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C571" s="13"/>
+      <c r="C571" s="14"/>
     </row>
     <row r="572" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C572" s="13"/>
+      <c r="C572" s="14"/>
     </row>
     <row r="573" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C573" s="13"/>
+      <c r="C573" s="14"/>
     </row>
     <row r="574" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C574" s="13"/>
+      <c r="C574" s="14"/>
     </row>
     <row r="575" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C575" s="13"/>
+      <c r="C575" s="14"/>
     </row>
     <row r="576" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C576" s="13"/>
+      <c r="C576" s="14"/>
     </row>
     <row r="577" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C577" s="13"/>
+      <c r="C577" s="14"/>
     </row>
     <row r="578" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C578" s="13"/>
+      <c r="C578" s="14"/>
     </row>
     <row r="579" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C579" s="13"/>
+      <c r="C579" s="14"/>
     </row>
     <row r="580" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C580" s="13"/>
+      <c r="C580" s="14"/>
     </row>
     <row r="581" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C581" s="13"/>
+      <c r="C581" s="14"/>
     </row>
     <row r="582" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C582" s="13"/>
+      <c r="C582" s="14"/>
     </row>
     <row r="583" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C583" s="13"/>
+      <c r="C583" s="14"/>
     </row>
     <row r="584" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C584" s="13"/>
+      <c r="C584" s="14"/>
     </row>
     <row r="585" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C585" s="13"/>
+      <c r="C585" s="14"/>
     </row>
     <row r="586" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C586" s="13"/>
+      <c r="C586" s="14"/>
     </row>
     <row r="587" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C587" s="13"/>
+      <c r="C587" s="14"/>
     </row>
     <row r="588" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C588" s="13"/>
+      <c r="C588" s="14"/>
     </row>
     <row r="589" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C589" s="13"/>
+      <c r="C589" s="14"/>
     </row>
     <row r="590" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C590" s="13"/>
+      <c r="C590" s="14"/>
     </row>
     <row r="591" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C591" s="13"/>
+      <c r="C591" s="14"/>
     </row>
     <row r="592" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C592" s="13"/>
+      <c r="C592" s="14"/>
     </row>
     <row r="593" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C593" s="13"/>
+      <c r="C593" s="14"/>
     </row>
     <row r="594" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C594" s="13"/>
+      <c r="C594" s="14"/>
     </row>
     <row r="595" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C595" s="13"/>
+      <c r="C595" s="14"/>
     </row>
     <row r="596" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C596" s="13"/>
+      <c r="C596" s="14"/>
     </row>
     <row r="597" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C597" s="13"/>
+      <c r="C597" s="14"/>
     </row>
     <row r="598" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C598" s="13"/>
+      <c r="C598" s="14"/>
     </row>
     <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C599" s="13"/>
+      <c r="C599" s="14"/>
     </row>
     <row r="600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C600" s="13"/>
+      <c r="C600" s="14"/>
     </row>
     <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C601" s="13"/>
+      <c r="C601" s="14"/>
     </row>
     <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C602" s="13"/>
+      <c r="C602" s="14"/>
     </row>
     <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C603" s="13"/>
+      <c r="C603" s="14"/>
     </row>
     <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C604" s="13"/>
+      <c r="C604" s="14"/>
     </row>
     <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C605" s="13"/>
+      <c r="C605" s="14"/>
     </row>
     <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C606" s="13"/>
+      <c r="C606" s="14"/>
     </row>
     <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C607" s="13"/>
+      <c r="C607" s="14"/>
     </row>
     <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C608" s="13"/>
+      <c r="C608" s="14"/>
     </row>
     <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C609" s="13"/>
+      <c r="C609" s="14"/>
     </row>
     <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C610" s="13"/>
+      <c r="C610" s="14"/>
     </row>
     <row r="611" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C611" s="13"/>
+      <c r="C611" s="14"/>
     </row>
     <row r="612" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C612" s="13"/>
+      <c r="C612" s="14"/>
     </row>
     <row r="613" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C613" s="13"/>
+      <c r="C613" s="14"/>
     </row>
     <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C614" s="13"/>
+      <c r="C614" s="14"/>
     </row>
     <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C615" s="13"/>
+      <c r="C615" s="14"/>
     </row>
     <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C616" s="13"/>
+      <c r="C616" s="14"/>
     </row>
     <row r="617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C617" s="13"/>
+      <c r="C617" s="14"/>
     </row>
     <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C618" s="13"/>
+      <c r="C618" s="14"/>
     </row>
     <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C619" s="13"/>
+      <c r="C619" s="14"/>
     </row>
     <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C620" s="13"/>
+      <c r="C620" s="14"/>
     </row>
     <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C621" s="13"/>
+      <c r="C621" s="14"/>
     </row>
     <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C622" s="13"/>
+      <c r="C622" s="14"/>
     </row>
     <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C623" s="13"/>
+      <c r="C623" s="14"/>
     </row>
     <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C624" s="13"/>
+      <c r="C624" s="14"/>
     </row>
     <row r="625" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C625" s="13"/>
+      <c r="C625" s="14"/>
     </row>
     <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C626" s="13"/>
+      <c r="C626" s="14"/>
     </row>
     <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C627" s="13"/>
+      <c r="C627" s="14"/>
     </row>
     <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C628" s="13"/>
+      <c r="C628" s="14"/>
     </row>
     <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C629" s="13"/>
+      <c r="C629" s="14"/>
     </row>
     <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C630" s="13"/>
+      <c r="C630" s="14"/>
     </row>
     <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C631" s="13"/>
+      <c r="C631" s="14"/>
     </row>
     <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C632" s="13"/>
+      <c r="C632" s="14"/>
     </row>
     <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C633" s="13"/>
+      <c r="C633" s="14"/>
     </row>
     <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C634" s="13"/>
+      <c r="C634" s="14"/>
     </row>
     <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C635" s="13"/>
+      <c r="C635" s="14"/>
     </row>
     <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C636" s="13"/>
+      <c r="C636" s="14"/>
     </row>
     <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C637" s="13"/>
+      <c r="C637" s="14"/>
     </row>
     <row r="638" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C638" s="13"/>
+      <c r="C638" s="14"/>
     </row>
     <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C639" s="13"/>
+      <c r="C639" s="14"/>
     </row>
     <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C640" s="13"/>
+      <c r="C640" s="14"/>
     </row>
     <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C641" s="13"/>
+      <c r="C641" s="14"/>
     </row>
     <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C642" s="13"/>
+      <c r="C642" s="14"/>
     </row>
     <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C643" s="13"/>
+      <c r="C643" s="14"/>
     </row>
     <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C644" s="13"/>
+      <c r="C644" s="14"/>
     </row>
     <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C645" s="13"/>
+      <c r="C645" s="14"/>
     </row>
     <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C646" s="13"/>
+      <c r="C646" s="14"/>
     </row>
     <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C647" s="13"/>
+      <c r="C647" s="14"/>
     </row>
     <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C648" s="13"/>
+      <c r="C648" s="14"/>
     </row>
     <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C649" s="13"/>
+      <c r="C649" s="14"/>
     </row>
     <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C650" s="13"/>
+      <c r="C650" s="14"/>
     </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C651" s="13"/>
+      <c r="C651" s="14"/>
     </row>
     <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C652" s="13"/>
+      <c r="C652" s="14"/>
     </row>
     <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C653" s="13"/>
+      <c r="C653" s="14"/>
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C654" s="13"/>
+      <c r="C654" s="14"/>
     </row>
     <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C655" s="13"/>
+      <c r="C655" s="14"/>
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C656" s="13"/>
+      <c r="C656" s="14"/>
     </row>
     <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C657" s="13"/>
+      <c r="C657" s="14"/>
     </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C658" s="13"/>
+      <c r="C658" s="14"/>
     </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C659" s="13"/>
+      <c r="C659" s="14"/>
     </row>
     <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C660" s="13"/>
+      <c r="C660" s="14"/>
     </row>
     <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C661" s="13"/>
+      <c r="C661" s="14"/>
     </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C662" s="13"/>
+      <c r="C662" s="14"/>
     </row>
     <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C663" s="13"/>
+      <c r="C663" s="14"/>
     </row>
     <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C664" s="13"/>
+      <c r="C664" s="14"/>
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C665" s="13"/>
+      <c r="C665" s="14"/>
     </row>
     <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C666" s="13"/>
+      <c r="C666" s="14"/>
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C667" s="13"/>
+      <c r="C667" s="14"/>
     </row>
     <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C668" s="13"/>
+      <c r="C668" s="14"/>
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C669" s="13"/>
+      <c r="C669" s="14"/>
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C670" s="13"/>
+      <c r="C670" s="14"/>
     </row>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C671" s="13"/>
+      <c r="C671" s="14"/>
     </row>
     <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C672" s="13"/>
+      <c r="C672" s="14"/>
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C673" s="13"/>
+      <c r="C673" s="14"/>
     </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C674" s="13"/>
+      <c r="C674" s="14"/>
     </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C675" s="13"/>
+      <c r="C675" s="14"/>
     </row>
     <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C676" s="13"/>
+      <c r="C676" s="14"/>
     </row>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C677" s="13"/>
+      <c r="C677" s="14"/>
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C678" s="13"/>
+      <c r="C678" s="14"/>
     </row>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C679" s="13"/>
+      <c r="C679" s="14"/>
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C680" s="13"/>
+      <c r="C680" s="14"/>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C681" s="13"/>
+      <c r="C681" s="14"/>
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C682" s="13"/>
+      <c r="C682" s="14"/>
     </row>
     <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C683" s="13"/>
+      <c r="C683" s="14"/>
     </row>
     <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C684" s="13"/>
+      <c r="C684" s="14"/>
     </row>
     <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C685" s="13"/>
+      <c r="C685" s="14"/>
     </row>
     <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C686" s="13"/>
+      <c r="C686" s="14"/>
     </row>
     <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C687" s="13"/>
+      <c r="C687" s="14"/>
     </row>
     <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C688" s="13"/>
+      <c r="C688" s="14"/>
     </row>
     <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C689" s="13"/>
+      <c r="C689" s="14"/>
     </row>
     <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C690" s="13"/>
+      <c r="C690" s="14"/>
     </row>
     <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C691" s="13"/>
+      <c r="C691" s="14"/>
     </row>
     <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C692" s="13"/>
+      <c r="C692" s="14"/>
     </row>
     <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C693" s="13"/>
+      <c r="C693" s="14"/>
     </row>
     <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C694" s="13"/>
+      <c r="C694" s="14"/>
     </row>
     <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C695" s="13"/>
+      <c r="C695" s="14"/>
     </row>
     <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C696" s="13"/>
+      <c r="C696" s="14"/>
     </row>
     <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C697" s="13"/>
+      <c r="C697" s="14"/>
     </row>
     <row r="698" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C698" s="13"/>
+      <c r="C698" s="14"/>
     </row>
     <row r="699" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C699" s="13"/>
+      <c r="C699" s="14"/>
     </row>
     <row r="700" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C700" s="13"/>
+      <c r="C700" s="14"/>
     </row>
     <row r="701" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C701" s="13"/>
+      <c r="C701" s="14"/>
     </row>
     <row r="702" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C702" s="13"/>
+      <c r="C702" s="14"/>
     </row>
     <row r="703" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C703" s="13"/>
+      <c r="C703" s="14"/>
     </row>
     <row r="704" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C704" s="13"/>
+      <c r="C704" s="14"/>
     </row>
     <row r="705" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C705" s="13"/>
+      <c r="C705" s="14"/>
     </row>
     <row r="706" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C706" s="13"/>
+      <c r="C706" s="14"/>
     </row>
     <row r="707" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C707" s="13"/>
+      <c r="C707" s="14"/>
     </row>
     <row r="708" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C708" s="13"/>
+      <c r="C708" s="14"/>
     </row>
     <row r="709" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C709" s="13"/>
+      <c r="C709" s="14"/>
     </row>
     <row r="710" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C710" s="13"/>
+      <c r="C710" s="14"/>
     </row>
     <row r="711" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C711" s="13"/>
+      <c r="C711" s="14"/>
     </row>
     <row r="712" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C712" s="13"/>
+      <c r="C712" s="14"/>
     </row>
     <row r="713" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C713" s="13"/>
+      <c r="C713" s="14"/>
     </row>
     <row r="714" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C714" s="13"/>
+      <c r="C714" s="14"/>
     </row>
     <row r="715" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C715" s="13"/>
+      <c r="C715" s="14"/>
     </row>
     <row r="716" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C716" s="13"/>
+      <c r="C716" s="14"/>
     </row>
     <row r="717" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C717" s="13"/>
+      <c r="C717" s="14"/>
     </row>
     <row r="718" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C718" s="13"/>
+      <c r="C718" s="14"/>
     </row>
     <row r="719" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C719" s="13"/>
+      <c r="C719" s="14"/>
     </row>
     <row r="720" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C720" s="13"/>
+      <c r="C720" s="14"/>
     </row>
     <row r="721" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C721" s="13"/>
+      <c r="C721" s="14"/>
     </row>
     <row r="722" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C722" s="13"/>
+      <c r="C722" s="14"/>
     </row>
     <row r="723" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C723" s="13"/>
+      <c r="C723" s="14"/>
     </row>
     <row r="724" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C724" s="13"/>
+      <c r="C724" s="14"/>
     </row>
     <row r="725" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C725" s="13"/>
+      <c r="C725" s="14"/>
     </row>
     <row r="726" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C726" s="13"/>
+      <c r="C726" s="14"/>
     </row>
     <row r="727" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C727" s="13"/>
+      <c r="C727" s="14"/>
     </row>
     <row r="728" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C728" s="13"/>
+      <c r="C728" s="14"/>
     </row>
     <row r="729" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C729" s="13"/>
+      <c r="C729" s="14"/>
     </row>
     <row r="730" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C730" s="13"/>
+      <c r="C730" s="14"/>
     </row>
     <row r="731" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C731" s="13"/>
+      <c r="C731" s="14"/>
     </row>
     <row r="732" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C732" s="13"/>
+      <c r="C732" s="14"/>
     </row>
     <row r="733" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C733" s="13"/>
+      <c r="C733" s="14"/>
     </row>
     <row r="734" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C734" s="13"/>
+      <c r="C734" s="14"/>
     </row>
     <row r="735" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C735" s="13"/>
+      <c r="C735" s="14"/>
     </row>
     <row r="736" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C736" s="13"/>
+      <c r="C736" s="14"/>
     </row>
     <row r="737" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C737" s="13"/>
+      <c r="C737" s="14"/>
     </row>
     <row r="738" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C738" s="13"/>
+      <c r="C738" s="14"/>
     </row>
     <row r="739" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C739" s="13"/>
+      <c r="C739" s="14"/>
     </row>
     <row r="740" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C740" s="13"/>
+      <c r="C740" s="14"/>
     </row>
     <row r="741" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C741" s="13"/>
+      <c r="C741" s="14"/>
     </row>
     <row r="742" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C742" s="13"/>
+      <c r="C742" s="14"/>
     </row>
     <row r="743" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C743" s="13"/>
+      <c r="C743" s="14"/>
     </row>
     <row r="744" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C744" s="13"/>
+      <c r="C744" s="14"/>
     </row>
     <row r="745" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C745" s="13"/>
+      <c r="C745" s="14"/>
     </row>
     <row r="746" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C746" s="13"/>
+      <c r="C746" s="14"/>
     </row>
     <row r="747" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C747" s="13"/>
+      <c r="C747" s="14"/>
     </row>
     <row r="748" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C748" s="13"/>
+      <c r="C748" s="14"/>
     </row>
     <row r="749" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C749" s="13"/>
+      <c r="C749" s="14"/>
     </row>
     <row r="750" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C750" s="13"/>
+      <c r="C750" s="14"/>
     </row>
     <row r="751" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C751" s="13"/>
+      <c r="C751" s="14"/>
     </row>
     <row r="752" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C752" s="13"/>
+      <c r="C752" s="14"/>
     </row>
     <row r="753" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C753" s="13"/>
+      <c r="C753" s="14"/>
     </row>
     <row r="754" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C754" s="13"/>
+      <c r="C754" s="14"/>
     </row>
     <row r="755" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C755" s="13"/>
+      <c r="C755" s="14"/>
     </row>
     <row r="756" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C756" s="13"/>
+      <c r="C756" s="14"/>
     </row>
     <row r="757" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C757" s="13"/>
+      <c r="C757" s="14"/>
     </row>
     <row r="758" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C758" s="13"/>
+      <c r="C758" s="14"/>
     </row>
     <row r="759" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C759" s="13"/>
+      <c r="C759" s="14"/>
     </row>
     <row r="760" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C760" s="13"/>
+      <c r="C760" s="14"/>
     </row>
     <row r="761" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C761" s="13"/>
+      <c r="C761" s="14"/>
     </row>
     <row r="762" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C762" s="13"/>
+      <c r="C762" s="14"/>
     </row>
     <row r="763" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C763" s="13"/>
+      <c r="C763" s="14"/>
     </row>
     <row r="764" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C764" s="13"/>
+      <c r="C764" s="14"/>
     </row>
     <row r="765" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C765" s="13"/>
+      <c r="C765" s="14"/>
     </row>
     <row r="766" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C766" s="13"/>
+      <c r="C766" s="14"/>
     </row>
     <row r="767" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C767" s="13"/>
+      <c r="C767" s="14"/>
     </row>
     <row r="768" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C768" s="13"/>
+      <c r="C768" s="14"/>
     </row>
     <row r="769" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C769" s="13"/>
+      <c r="C769" s="14"/>
     </row>
     <row r="770" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C770" s="13"/>
+      <c r="C770" s="14"/>
     </row>
     <row r="771" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C771" s="13"/>
+      <c r="C771" s="14"/>
     </row>
     <row r="772" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C772" s="13"/>
+      <c r="C772" s="14"/>
     </row>
     <row r="773" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C773" s="13"/>
+      <c r="C773" s="14"/>
     </row>
     <row r="774" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C774" s="13"/>
+      <c r="C774" s="14"/>
     </row>
     <row r="775" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C775" s="13"/>
+      <c r="C775" s="14"/>
     </row>
     <row r="776" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C776" s="13"/>
+      <c r="C776" s="14"/>
     </row>
     <row r="777" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C777" s="13"/>
+      <c r="C777" s="14"/>
     </row>
     <row r="778" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C778" s="13"/>
+      <c r="C778" s="14"/>
     </row>
     <row r="779" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C779" s="13"/>
+      <c r="C779" s="14"/>
     </row>
     <row r="780" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C780" s="13"/>
+      <c r="C780" s="14"/>
     </row>
     <row r="781" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C781" s="13"/>
+      <c r="C781" s="14"/>
     </row>
     <row r="782" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C782" s="13"/>
+      <c r="C782" s="14"/>
     </row>
     <row r="783" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C783" s="13"/>
+      <c r="C783" s="14"/>
     </row>
     <row r="784" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C784" s="13"/>
+      <c r="C784" s="14"/>
     </row>
     <row r="785" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C785" s="13"/>
+      <c r="C785" s="14"/>
     </row>
     <row r="786" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C786" s="13"/>
+      <c r="C786" s="14"/>
     </row>
     <row r="787" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C787" s="13"/>
+      <c r="C787" s="14"/>
     </row>
     <row r="788" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C788" s="13"/>
+      <c r="C788" s="14"/>
     </row>
     <row r="789" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C789" s="13"/>
+      <c r="C789" s="14"/>
     </row>
     <row r="790" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C790" s="13"/>
+      <c r="C790" s="14"/>
     </row>
     <row r="791" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C791" s="13"/>
+      <c r="C791" s="14"/>
     </row>
     <row r="792" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C792" s="13"/>
+      <c r="C792" s="14"/>
     </row>
     <row r="793" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C793" s="13"/>
+      <c r="C793" s="14"/>
     </row>
     <row r="794" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C794" s="13"/>
+      <c r="C794" s="14"/>
     </row>
     <row r="795" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C795" s="13"/>
+      <c r="C795" s="14"/>
     </row>
     <row r="796" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C796" s="13"/>
+      <c r="C796" s="14"/>
     </row>
     <row r="797" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C797" s="13"/>
+      <c r="C797" s="14"/>
     </row>
     <row r="798" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C798" s="13"/>
+      <c r="C798" s="14"/>
     </row>
     <row r="799" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C799" s="13"/>
+      <c r="C799" s="14"/>
     </row>
     <row r="800" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C800" s="13"/>
+      <c r="C800" s="14"/>
     </row>
     <row r="801" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C801" s="13"/>
+      <c r="C801" s="14"/>
     </row>
     <row r="802" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C802" s="13"/>
+      <c r="C802" s="14"/>
     </row>
     <row r="803" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C803" s="13"/>
+      <c r="C803" s="14"/>
     </row>
     <row r="804" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C804" s="13"/>
+      <c r="C804" s="14"/>
     </row>
     <row r="805" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C805" s="13"/>
+      <c r="C805" s="14"/>
     </row>
     <row r="806" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C806" s="13"/>
+      <c r="C806" s="14"/>
     </row>
     <row r="807" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C807" s="13"/>
+      <c r="C807" s="14"/>
     </row>
     <row r="808" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C808" s="13"/>
+      <c r="C808" s="14"/>
     </row>
     <row r="809" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C809" s="13"/>
+      <c r="C809" s="14"/>
     </row>
     <row r="810" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C810" s="13"/>
+      <c r="C810" s="14"/>
     </row>
     <row r="811" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C811" s="13"/>
+      <c r="C811" s="14"/>
     </row>
     <row r="812" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C812" s="13"/>
+      <c r="C812" s="14"/>
     </row>
     <row r="813" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C813" s="13"/>
+      <c r="C813" s="14"/>
     </row>
     <row r="814" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C814" s="13"/>
+      <c r="C814" s="14"/>
     </row>
     <row r="815" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C815" s="13"/>
+      <c r="C815" s="14"/>
     </row>
     <row r="816" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C816" s="13"/>
+      <c r="C816" s="14"/>
     </row>
     <row r="817" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C817" s="13"/>
+      <c r="C817" s="14"/>
     </row>
     <row r="818" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C818" s="13"/>
+      <c r="C818" s="14"/>
     </row>
     <row r="819" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C819" s="13"/>
+      <c r="C819" s="14"/>
     </row>
     <row r="820" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C820" s="13"/>
+      <c r="C820" s="14"/>
     </row>
     <row r="821" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C821" s="13"/>
+      <c r="C821" s="14"/>
     </row>
     <row r="822" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C822" s="13"/>
+      <c r="C822" s="14"/>
     </row>
     <row r="823" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C823" s="13"/>
+      <c r="C823" s="14"/>
     </row>
     <row r="824" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C824" s="13"/>
+      <c r="C824" s="14"/>
     </row>
     <row r="825" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C825" s="13"/>
+      <c r="C825" s="14"/>
     </row>
     <row r="826" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C826" s="13"/>
+      <c r="C826" s="14"/>
     </row>
     <row r="827" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C827" s="13"/>
+      <c r="C827" s="14"/>
     </row>
     <row r="828" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C828" s="13"/>
+      <c r="C828" s="14"/>
     </row>
     <row r="829" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C829" s="13"/>
+      <c r="C829" s="14"/>
     </row>
     <row r="830" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C830" s="13"/>
+      <c r="C830" s="14"/>
     </row>
     <row r="831" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C831" s="13"/>
+      <c r="C831" s="14"/>
     </row>
     <row r="832" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C832" s="13"/>
+      <c r="C832" s="14"/>
     </row>
     <row r="833" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C833" s="13"/>
+      <c r="C833" s="14"/>
     </row>
     <row r="834" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C834" s="13"/>
+      <c r="C834" s="14"/>
     </row>
     <row r="835" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C835" s="13"/>
+      <c r="C835" s="14"/>
     </row>
     <row r="836" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C836" s="13"/>
+      <c r="C836" s="14"/>
     </row>
     <row r="837" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C837" s="13"/>
+      <c r="C837" s="14"/>
     </row>
     <row r="838" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C838" s="13"/>
+      <c r="C838" s="14"/>
     </row>
     <row r="839" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C839" s="13"/>
+      <c r="C839" s="14"/>
     </row>
     <row r="840" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C840" s="13"/>
+      <c r="C840" s="14"/>
     </row>
     <row r="841" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C841" s="13"/>
+      <c r="C841" s="14"/>
     </row>
     <row r="842" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C842" s="13"/>
+      <c r="C842" s="14"/>
     </row>
     <row r="843" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C843" s="13"/>
+      <c r="C843" s="14"/>
     </row>
     <row r="844" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C844" s="13"/>
+      <c r="C844" s="14"/>
     </row>
     <row r="845" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C845" s="13"/>
+      <c r="C845" s="14"/>
     </row>
     <row r="846" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C846" s="13"/>
+      <c r="C846" s="14"/>
     </row>
     <row r="847" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C847" s="13"/>
+      <c r="C847" s="14"/>
     </row>
     <row r="848" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C848" s="13"/>
+      <c r="C848" s="14"/>
     </row>
     <row r="849" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C849" s="13"/>
+      <c r="C849" s="14"/>
     </row>
     <row r="850" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C850" s="13"/>
+      <c r="C850" s="14"/>
     </row>
     <row r="851" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C851" s="13"/>
+      <c r="C851" s="14"/>
     </row>
     <row r="852" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C852" s="13"/>
+      <c r="C852" s="14"/>
     </row>
     <row r="853" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C853" s="13"/>
+      <c r="C853" s="14"/>
     </row>
     <row r="854" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C854" s="13"/>
+      <c r="C854" s="14"/>
     </row>
     <row r="855" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C855" s="13"/>
+      <c r="C855" s="14"/>
     </row>
     <row r="856" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C856" s="13"/>
+      <c r="C856" s="14"/>
     </row>
     <row r="857" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C857" s="13"/>
+      <c r="C857" s="14"/>
     </row>
     <row r="858" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C858" s="13"/>
+      <c r="C858" s="14"/>
     </row>
     <row r="859" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C859" s="13"/>
+      <c r="C859" s="14"/>
     </row>
     <row r="860" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C860" s="13"/>
+      <c r="C860" s="14"/>
     </row>
     <row r="861" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C861" s="13"/>
+      <c r="C861" s="14"/>
     </row>
     <row r="862" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C862" s="13"/>
+      <c r="C862" s="14"/>
     </row>
     <row r="863" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C863" s="13"/>
+      <c r="C863" s="14"/>
     </row>
     <row r="864" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C864" s="13"/>
+      <c r="C864" s="14"/>
     </row>
     <row r="865" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C865" s="13"/>
+      <c r="C865" s="14"/>
     </row>
     <row r="866" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C866" s="13"/>
+      <c r="C866" s="14"/>
     </row>
     <row r="867" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C867" s="13"/>
+      <c r="C867" s="14"/>
     </row>
     <row r="868" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C868" s="13"/>
+      <c r="C868" s="14"/>
     </row>
     <row r="869" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C869" s="13"/>
+      <c r="C869" s="14"/>
     </row>
     <row r="870" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C870" s="13"/>
+      <c r="C870" s="14"/>
     </row>
     <row r="871" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C871" s="13"/>
+      <c r="C871" s="14"/>
     </row>
     <row r="872" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C872" s="13"/>
+      <c r="C872" s="14"/>
     </row>
     <row r="873" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C873" s="13"/>
+      <c r="C873" s="14"/>
     </row>
     <row r="874" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C874" s="13"/>
+      <c r="C874" s="14"/>
     </row>
     <row r="875" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C875" s="13"/>
+      <c r="C875" s="14"/>
     </row>
     <row r="876" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C876" s="13"/>
+      <c r="C876" s="14"/>
     </row>
     <row r="877" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C877" s="13"/>
+      <c r="C877" s="14"/>
     </row>
     <row r="878" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C878" s="13"/>
+      <c r="C878" s="14"/>
     </row>
     <row r="879" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C879" s="13"/>
+      <c r="C879" s="14"/>
     </row>
     <row r="880" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C880" s="13"/>
+      <c r="C880" s="14"/>
     </row>
     <row r="881" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C881" s="13"/>
+      <c r="C881" s="14"/>
     </row>
     <row r="882" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C882" s="13"/>
+      <c r="C882" s="14"/>
     </row>
     <row r="883" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C883" s="13"/>
+      <c r="C883" s="14"/>
     </row>
     <row r="884" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C884" s="13"/>
+      <c r="C884" s="14"/>
     </row>
     <row r="885" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C885" s="13"/>
+      <c r="C885" s="14"/>
     </row>
     <row r="886" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C886" s="13"/>
+      <c r="C886" s="14"/>
     </row>
     <row r="887" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C887" s="13"/>
+      <c r="C887" s="14"/>
     </row>
     <row r="888" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C888" s="13"/>
+      <c r="C888" s="14"/>
     </row>
     <row r="889" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C889" s="13"/>
+      <c r="C889" s="14"/>
     </row>
     <row r="890" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C890" s="13"/>
+      <c r="C890" s="14"/>
     </row>
     <row r="891" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C891" s="13"/>
+      <c r="C891" s="14"/>
     </row>
     <row r="892" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C892" s="13"/>
+      <c r="C892" s="14"/>
     </row>
     <row r="893" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C893" s="13"/>
+      <c r="C893" s="14"/>
     </row>
     <row r="894" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C894" s="13"/>
+      <c r="C894" s="14"/>
     </row>
     <row r="895" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C895" s="13"/>
+      <c r="C895" s="14"/>
     </row>
     <row r="896" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C896" s="13"/>
+      <c r="C896" s="14"/>
     </row>
     <row r="897" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C897" s="13"/>
+      <c r="C897" s="14"/>
     </row>
     <row r="898" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C898" s="13"/>
+      <c r="C898" s="14"/>
     </row>
     <row r="899" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C899" s="13"/>
+      <c r="C899" s="14"/>
     </row>
     <row r="900" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C900" s="13"/>
+      <c r="C900" s="14"/>
     </row>
     <row r="901" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C901" s="13"/>
+      <c r="C901" s="14"/>
     </row>
     <row r="902" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C902" s="13"/>
+      <c r="C902" s="14"/>
     </row>
     <row r="903" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C903" s="13"/>
+      <c r="C903" s="14"/>
     </row>
     <row r="904" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C904" s="13"/>
+      <c r="C904" s="14"/>
     </row>
     <row r="905" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C905" s="13"/>
+      <c r="C905" s="14"/>
     </row>
     <row r="906" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C906" s="13"/>
+      <c r="C906" s="14"/>
     </row>
     <row r="907" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C907" s="13"/>
+      <c r="C907" s="14"/>
     </row>
     <row r="908" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C908" s="13"/>
+      <c r="C908" s="14"/>
     </row>
     <row r="909" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C909" s="13"/>
+      <c r="C909" s="14"/>
     </row>
     <row r="910" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C910" s="13"/>
+      <c r="C910" s="14"/>
     </row>
     <row r="911" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C911" s="13"/>
+      <c r="C911" s="14"/>
     </row>
     <row r="912" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C912" s="13"/>
+      <c r="C912" s="14"/>
     </row>
     <row r="913" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C913" s="13"/>
+      <c r="C913" s="14"/>
     </row>
     <row r="914" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C914" s="13"/>
+      <c r="C914" s="14"/>
     </row>
     <row r="915" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C915" s="13"/>
+      <c r="C915" s="14"/>
     </row>
     <row r="916" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C916" s="13"/>
+      <c r="C916" s="14"/>
     </row>
     <row r="917" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C917" s="13"/>
+      <c r="C917" s="14"/>
     </row>
     <row r="918" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C918" s="13"/>
+      <c r="C918" s="14"/>
     </row>
     <row r="919" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C919" s="13"/>
+      <c r="C919" s="14"/>
     </row>
     <row r="920" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C920" s="13"/>
+      <c r="C920" s="14"/>
     </row>
     <row r="921" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C921" s="13"/>
+      <c r="C921" s="14"/>
     </row>
     <row r="922" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C922" s="13"/>
+      <c r="C922" s="14"/>
     </row>
     <row r="923" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C923" s="13"/>
+      <c r="C923" s="14"/>
     </row>
     <row r="924" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C924" s="13"/>
+      <c r="C924" s="14"/>
     </row>
     <row r="925" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C925" s="13"/>
+      <c r="C925" s="14"/>
     </row>
     <row r="926" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C926" s="13"/>
+      <c r="C926" s="14"/>
     </row>
     <row r="927" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C927" s="13"/>
+      <c r="C927" s="14"/>
     </row>
     <row r="928" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C928" s="13"/>
+      <c r="C928" s="14"/>
     </row>
     <row r="929" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C929" s="13"/>
+      <c r="C929" s="14"/>
     </row>
     <row r="930" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C930" s="13"/>
+      <c r="C930" s="14"/>
     </row>
     <row r="931" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C931" s="13"/>
+      <c r="C931" s="14"/>
     </row>
     <row r="932" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C932" s="13"/>
+      <c r="C932" s="14"/>
     </row>
     <row r="933" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C933" s="13"/>
+      <c r="C933" s="14"/>
     </row>
     <row r="934" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C934" s="13"/>
+      <c r="C934" s="14"/>
     </row>
     <row r="935" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C935" s="13"/>
+      <c r="C935" s="14"/>
     </row>
     <row r="936" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C936" s="13"/>
+      <c r="C936" s="14"/>
     </row>
     <row r="937" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C937" s="13"/>
+      <c r="C937" s="14"/>
     </row>
     <row r="938" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C938" s="13"/>
+      <c r="C938" s="14"/>
     </row>
     <row r="939" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C939" s="13"/>
+      <c r="C939" s="14"/>
     </row>
     <row r="940" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C940" s="13"/>
+      <c r="C940" s="14"/>
     </row>
     <row r="941" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C941" s="13"/>
+      <c r="C941" s="14"/>
     </row>
     <row r="942" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C942" s="13"/>
+      <c r="C942" s="14"/>
     </row>
     <row r="943" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C943" s="13"/>
+      <c r="C943" s="14"/>
     </row>
     <row r="944" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C944" s="13"/>
+      <c r="C944" s="14"/>
     </row>
     <row r="945" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C945" s="13"/>
+      <c r="C945" s="14"/>
     </row>
     <row r="946" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C946" s="13"/>
+      <c r="C946" s="14"/>
     </row>
     <row r="947" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C947" s="13"/>
+      <c r="C947" s="14"/>
     </row>
     <row r="948" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C948" s="13"/>
+      <c r="C948" s="14"/>
     </row>
     <row r="949" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C949" s="13"/>
+      <c r="C949" s="14"/>
     </row>
     <row r="950" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C950" s="13"/>
+      <c r="C950" s="14"/>
     </row>
     <row r="951" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C951" s="13"/>
+      <c r="C951" s="14"/>
     </row>
     <row r="952" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C952" s="13"/>
+      <c r="C952" s="14"/>
     </row>
     <row r="953" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C953" s="13"/>
+      <c r="C953" s="14"/>
     </row>
     <row r="954" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C954" s="13"/>
+      <c r="C954" s="14"/>
     </row>
     <row r="955" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C955" s="13"/>
+      <c r="C955" s="14"/>
     </row>
     <row r="956" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C956" s="13"/>
+      <c r="C956" s="14"/>
     </row>
     <row r="957" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C957" s="13"/>
+      <c r="C957" s="14"/>
     </row>
     <row r="958" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C958" s="13"/>
+      <c r="C958" s="14"/>
     </row>
     <row r="959" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C959" s="13"/>
+      <c r="C959" s="14"/>
     </row>
     <row r="960" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C960" s="13"/>
+      <c r="C960" s="14"/>
     </row>
     <row r="961" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C961" s="13"/>
+      <c r="C961" s="14"/>
     </row>
     <row r="962" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C962" s="13"/>
+      <c r="C962" s="14"/>
     </row>
     <row r="963" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C963" s="13"/>
+      <c r="C963" s="14"/>
     </row>
     <row r="964" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C964" s="13"/>
+      <c r="C964" s="14"/>
     </row>
     <row r="965" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C965" s="13"/>
+      <c r="C965" s="14"/>
     </row>
     <row r="966" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C966" s="13"/>
+      <c r="C966" s="14"/>
     </row>
     <row r="967" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C967" s="13"/>
+      <c r="C967" s="14"/>
     </row>
     <row r="968" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C968" s="13"/>
+      <c r="C968" s="14"/>
     </row>
     <row r="969" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C969" s="13"/>
+      <c r="C969" s="14"/>
     </row>
     <row r="970" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C970" s="13"/>
+      <c r="C970" s="14"/>
     </row>
     <row r="971" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C971" s="13"/>
+      <c r="C971" s="14"/>
     </row>
     <row r="972" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C972" s="13"/>
+      <c r="C972" s="14"/>
     </row>
     <row r="973" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C973" s="13"/>
+      <c r="C973" s="14"/>
     </row>
     <row r="974" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C974" s="13"/>
+      <c r="C974" s="14"/>
     </row>
     <row r="975" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C975" s="13"/>
+      <c r="C975" s="14"/>
     </row>
     <row r="976" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C976" s="13"/>
+      <c r="C976" s="14"/>
     </row>
     <row r="977" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C977" s="13"/>
+      <c r="C977" s="14"/>
     </row>
     <row r="978" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C978" s="13"/>
+      <c r="C978" s="14"/>
     </row>
     <row r="979" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C979" s="13"/>
+      <c r="C979" s="14"/>
     </row>
     <row r="980" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C980" s="13"/>
+      <c r="C980" s="14"/>
     </row>
     <row r="981" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C981" s="13"/>
+      <c r="C981" s="14"/>
     </row>
     <row r="982" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C982" s="13"/>
+      <c r="C982" s="14"/>
     </row>
     <row r="983" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C983" s="13"/>
+      <c r="C983" s="14"/>
     </row>
     <row r="984" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C984" s="13"/>
+      <c r="C984" s="14"/>
     </row>
     <row r="985" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C985" s="13"/>
+      <c r="C985" s="14"/>
     </row>
     <row r="986" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C986" s="13"/>
+      <c r="C986" s="14"/>
     </row>
     <row r="987" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C987" s="13"/>
+      <c r="C987" s="14"/>
     </row>
     <row r="988" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C988" s="13"/>
+      <c r="C988" s="14"/>
     </row>
     <row r="989" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C989" s="13"/>
+      <c r="C989" s="14"/>
     </row>
     <row r="990" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C990" s="13"/>
+      <c r="C990" s="14"/>
     </row>
     <row r="991" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C991" s="13"/>
+      <c r="C991" s="14"/>
     </row>
     <row r="992" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C992" s="13"/>
+      <c r="C992" s="14"/>
     </row>
     <row r="993" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C993" s="13"/>
+      <c r="C993" s="14"/>
     </row>
     <row r="994" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C994" s="13"/>
+      <c r="C994" s="14"/>
     </row>
     <row r="995" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C995" s="13"/>
+      <c r="C995" s="14"/>
     </row>
     <row r="996" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C996" s="13"/>
+      <c r="C996" s="14"/>
     </row>
     <row r="997" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C997" s="13"/>
+      <c r="C997" s="14"/>
     </row>
     <row r="998" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C998" s="13"/>
+      <c r="C998" s="14"/>
     </row>
     <row r="999" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C999" s="13"/>
+      <c r="C999" s="14"/>
     </row>
     <row r="1000" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1000" s="13"/>
+      <c r="C1000" s="14"/>
     </row>
     <row r="1001" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1001" s="13"/>
+      <c r="C1001" s="14"/>
     </row>
     <row r="1002" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1002" s="13"/>
+      <c r="C1002" s="14"/>
     </row>
     <row r="1003" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1003" s="13"/>
+      <c r="C1003" s="14"/>
     </row>
     <row r="1004" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1004" s="13"/>
+      <c r="C1004" s="14"/>
     </row>
     <row r="1005" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1005" s="13"/>
+      <c r="C1005" s="14"/>
     </row>
     <row r="1006" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1006" s="13"/>
+      <c r="C1006" s="14"/>
     </row>
     <row r="1007" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1007" s="13"/>
+      <c r="C1007" s="14"/>
     </row>
     <row r="1008" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C1008" s="13"/>
+      <c r="C1008" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>